<commit_message>
Script de criacao + Modelo Fisico + atualizacao tabelas validacao
</commit_message>
<xml_diff>
--- a/Banco de Dados/SPMedGroup_TabelasValidacao.xlsx
+++ b/Banco de Dados/SPMedGroup_TabelasValidacao.xlsx
@@ -152,9 +152,6 @@
     <t>carlos@email.com</t>
   </si>
   <si>
-    <t>comum</t>
-  </si>
-  <si>
     <t>Maria Lúcia Silva</t>
   </si>
   <si>
@@ -200,18 +197,12 @@
     <t>Homem transgênero</t>
   </si>
   <si>
-    <t>Gênero</t>
-  </si>
-  <si>
     <t>49kg</t>
   </si>
   <si>
     <t>Teve dengue há 15 dias</t>
   </si>
   <si>
-    <t>USUARIO_TIPO</t>
-  </si>
-  <si>
     <t>administrador</t>
   </si>
   <si>
@@ -234,6 +225,15 @@
   </si>
   <si>
     <t>GÊNEROS</t>
+  </si>
+  <si>
+    <t>USUARIOS_TIPOS</t>
+  </si>
+  <si>
+    <t>Id_Gênero</t>
+  </si>
+  <si>
+    <t>médico</t>
   </si>
 </sst>
 </file>
@@ -693,15 +693,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -721,21 +712,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -767,19 +743,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -819,6 +786,39 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1104,8 +1104,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:H5"/>
+    <sheetView tabSelected="1" topLeftCell="F19" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1124,22 +1124,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="25"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="50"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="18" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>1</v>
@@ -1151,14 +1151,14 @@
         <v>3</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="H2" s="27" t="s">
-        <v>65</v>
+        <v>61</v>
+      </c>
+      <c r="H2" s="19" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B3" s="28">
+      <c r="B3" s="20">
         <v>1</v>
       </c>
       <c r="C3" s="8" t="s">
@@ -1174,118 +1174,118 @@
         <v>0</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="H3" s="58" t="s">
-        <v>67</v>
+        <v>65</v>
+      </c>
+      <c r="H3" s="47" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B4" s="28"/>
+      <c r="B4" s="20"/>
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
       <c r="G4" s="8"/>
-      <c r="H4" s="29"/>
+      <c r="H4" s="21"/>
     </row>
     <row r="5" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="30"/>
-      <c r="C5" s="31"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="31"/>
-      <c r="F5" s="31"/>
-      <c r="G5" s="31"/>
-      <c r="H5" s="33"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="25"/>
     </row>
     <row r="6" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B7" s="21" t="s">
+      <c r="B7" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="22"/>
-      <c r="E7" s="11" t="s">
+      <c r="C7" s="54"/>
+      <c r="E7" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="13"/>
-      <c r="H7" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="I7" s="13"/>
+      <c r="F7" s="52"/>
+      <c r="H7" s="51" t="s">
+        <v>67</v>
+      </c>
+      <c r="I7" s="52"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="E8" s="14" t="s">
+      <c r="E8" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="15" t="s">
+      <c r="F8" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="H8" s="14" t="s">
+      <c r="H8" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="I8" s="15" t="s">
-        <v>0</v>
+      <c r="I8" s="12" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B9" s="16">
-        <v>1</v>
-      </c>
-      <c r="C9" s="17" t="s">
+      <c r="B9" s="13">
+        <v>1</v>
+      </c>
+      <c r="C9" s="14" t="s">
         <v>39</v>
       </c>
       <c r="D9" s="1"/>
-      <c r="E9" s="16">
-        <v>1</v>
-      </c>
-      <c r="F9" s="17" t="s">
+      <c r="E9" s="13">
+        <v>1</v>
+      </c>
+      <c r="F9" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="H9" s="16">
-        <v>1</v>
-      </c>
-      <c r="I9" s="17" t="s">
-        <v>62</v>
+      <c r="H9" s="13">
+        <v>1</v>
+      </c>
+      <c r="I9" s="14" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="18"/>
-      <c r="C10" s="20"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="17"/>
       <c r="D10" s="1"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="20"/>
-      <c r="H10" s="18">
+      <c r="E10" s="15"/>
+      <c r="F10" s="17"/>
+      <c r="H10" s="15">
         <v>2</v>
       </c>
-      <c r="I10" s="20" t="s">
-        <v>42</v>
+      <c r="I10" s="17" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="23" t="s">
+      <c r="A12" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="24"/>
-      <c r="C12" s="24"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="25"/>
-      <c r="H12" s="23" t="s">
+      <c r="B12" s="49"/>
+      <c r="C12" s="49"/>
+      <c r="D12" s="49"/>
+      <c r="E12" s="49"/>
+      <c r="F12" s="50"/>
+      <c r="H12" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="I12" s="24"/>
-      <c r="J12" s="24"/>
-      <c r="K12" s="25"/>
+      <c r="I12" s="49"/>
+      <c r="J12" s="49"/>
+      <c r="K12" s="50"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" s="26" t="s">
+      <c r="A13" s="18" t="s">
         <v>5</v>
       </c>
       <c r="B13" s="5" t="s">
@@ -1300,10 +1300,10 @@
       <c r="E13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F13" s="27" t="s">
+      <c r="F13" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="H13" s="26" t="s">
+      <c r="H13" s="18" t="s">
         <v>5</v>
       </c>
       <c r="I13" s="5" t="s">
@@ -1312,12 +1312,12 @@
       <c r="J13" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="K13" s="27" t="s">
-        <v>63</v>
+      <c r="K13" s="19" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" s="28">
+      <c r="A14" s="20">
         <v>1</v>
       </c>
       <c r="B14" s="8" t="s">
@@ -1332,10 +1332,10 @@
       <c r="E14" s="8">
         <v>1</v>
       </c>
-      <c r="F14" s="29">
-        <v>1</v>
-      </c>
-      <c r="H14" s="28">
+      <c r="F14" s="21">
+        <v>1</v>
+      </c>
+      <c r="H14" s="20">
         <v>1</v>
       </c>
       <c r="I14" s="7" t="s">
@@ -1344,41 +1344,41 @@
       <c r="J14" s="8">
         <v>1234</v>
       </c>
-      <c r="K14" s="29">
+      <c r="K14" s="21">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15" s="28"/>
+      <c r="A15" s="20"/>
       <c r="B15" s="8"/>
       <c r="C15" s="6"/>
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
-      <c r="F15" s="29"/>
-      <c r="H15" s="28">
+      <c r="F15" s="21"/>
+      <c r="H15" s="20">
         <v>2</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J15" s="8">
         <v>4321</v>
       </c>
-      <c r="K15" s="29">
+      <c r="K15" s="21">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="30"/>
-      <c r="B16" s="31"/>
-      <c r="C16" s="32"/>
-      <c r="D16" s="31"/>
-      <c r="E16" s="31"/>
-      <c r="F16" s="33"/>
-      <c r="H16" s="34"/>
-      <c r="I16" s="31"/>
-      <c r="J16" s="31"/>
-      <c r="K16" s="33"/>
+      <c r="A16" s="22"/>
+      <c r="B16" s="23"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="25"/>
+      <c r="H16" s="26"/>
+      <c r="I16" s="23"/>
+      <c r="J16" s="23"/>
+      <c r="K16" s="25"/>
     </row>
     <row r="17" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="9"/>
@@ -1386,24 +1386,24 @@
       <c r="D17" s="9"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A18" s="37" t="s">
+      <c r="A18" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="40"/>
-      <c r="C18" s="40"/>
-      <c r="D18" s="40"/>
-      <c r="E18" s="40"/>
-      <c r="F18" s="40"/>
-      <c r="G18" s="40"/>
-      <c r="H18" s="40"/>
-      <c r="I18" s="40"/>
-      <c r="J18" s="41"/>
+      <c r="B18" s="57"/>
+      <c r="C18" s="57"/>
+      <c r="D18" s="57"/>
+      <c r="E18" s="57"/>
+      <c r="F18" s="57"/>
+      <c r="G18" s="57"/>
+      <c r="H18" s="57"/>
+      <c r="I18" s="57"/>
+      <c r="J18" s="58"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A19" s="26" t="s">
+      <c r="A19" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="B19" s="38" t="s">
+      <c r="B19" s="29" t="s">
         <v>0</v>
       </c>
       <c r="C19" s="2" t="s">
@@ -1427,180 +1427,180 @@
       <c r="I19" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="J19" s="15" t="s">
+      <c r="J19" s="12" t="s">
         <v>18</v>
       </c>
       <c r="K19" s="1"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A20" s="28">
-        <v>1</v>
-      </c>
-      <c r="B20" s="39" t="s">
-        <v>43</v>
+      <c r="A20" s="20">
+        <v>1</v>
+      </c>
+      <c r="B20" s="30" t="s">
+        <v>42</v>
       </c>
       <c r="C20" s="3">
         <v>2</v>
       </c>
       <c r="D20" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E20" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="F20" s="37">
+        <v>40280</v>
+      </c>
+      <c r="G20" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="F20" s="48">
-        <v>40280</v>
-      </c>
-      <c r="G20" s="3" t="s">
+      <c r="H20" s="3" t="s">
         <v>47</v>
-      </c>
-      <c r="H20" s="3" t="s">
-        <v>48</v>
       </c>
       <c r="I20" s="3">
         <v>84893303003</v>
       </c>
-      <c r="J20" s="17">
+      <c r="J20" s="14">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A21" s="42"/>
-      <c r="B21" s="39"/>
-      <c r="C21" s="43"/>
-      <c r="D21" s="43"/>
-      <c r="E21" s="43"/>
-      <c r="F21" s="43"/>
-      <c r="G21" s="43"/>
-      <c r="H21" s="43"/>
-      <c r="I21" s="43"/>
-      <c r="J21" s="44"/>
+      <c r="A21" s="31"/>
+      <c r="B21" s="30"/>
+      <c r="C21" s="32"/>
+      <c r="D21" s="32"/>
+      <c r="E21" s="32"/>
+      <c r="F21" s="32"/>
+      <c r="G21" s="32"/>
+      <c r="H21" s="32"/>
+      <c r="I21" s="32"/>
+      <c r="J21" s="33"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A22" s="42"/>
-      <c r="B22" s="39"/>
-      <c r="C22" s="43"/>
-      <c r="D22" s="43"/>
-      <c r="E22" s="43"/>
-      <c r="F22" s="43"/>
-      <c r="G22" s="43"/>
-      <c r="H22" s="43"/>
-      <c r="I22" s="43"/>
-      <c r="J22" s="44"/>
+      <c r="A22" s="31"/>
+      <c r="B22" s="30"/>
+      <c r="C22" s="32"/>
+      <c r="D22" s="32"/>
+      <c r="E22" s="32"/>
+      <c r="F22" s="32"/>
+      <c r="G22" s="32"/>
+      <c r="H22" s="32"/>
+      <c r="I22" s="32"/>
+      <c r="J22" s="33"/>
     </row>
     <row r="23" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="45"/>
-      <c r="B23" s="57"/>
-      <c r="C23" s="46"/>
-      <c r="D23" s="46"/>
-      <c r="E23" s="46"/>
-      <c r="F23" s="46"/>
-      <c r="G23" s="46"/>
-      <c r="H23" s="46"/>
-      <c r="I23" s="46"/>
-      <c r="J23" s="47"/>
+      <c r="A23" s="34"/>
+      <c r="B23" s="46"/>
+      <c r="C23" s="35"/>
+      <c r="D23" s="35"/>
+      <c r="E23" s="35"/>
+      <c r="F23" s="35"/>
+      <c r="G23" s="35"/>
+      <c r="H23" s="35"/>
+      <c r="I23" s="35"/>
+      <c r="J23" s="36"/>
     </row>
     <row r="24" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B25" s="21" t="s">
+      <c r="B25" s="53" t="s">
         <v>19</v>
       </c>
-      <c r="C25" s="22"/>
-      <c r="E25" s="23" t="s">
-        <v>69</v>
-      </c>
-      <c r="F25" s="25"/>
+      <c r="C25" s="54"/>
+      <c r="E25" s="48" t="s">
+        <v>66</v>
+      </c>
+      <c r="F25" s="50"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B26" s="14" t="s">
+      <c r="B26" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C26" s="15" t="s">
+      <c r="C26" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="E26" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="F26" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="E26" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="F26" s="27" t="s">
-        <v>34</v>
-      </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B27" s="16">
-        <v>1</v>
-      </c>
-      <c r="C27" s="17" t="s">
+      <c r="B27" s="13">
+        <v>1</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="E27" s="20">
+        <v>1</v>
+      </c>
+      <c r="F27" s="21" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B28" s="38">
+        <v>2</v>
+      </c>
+      <c r="C28" s="45" t="s">
         <v>49</v>
       </c>
-      <c r="E27" s="28">
-        <v>1</v>
-      </c>
-      <c r="F27" s="29" t="s">
+      <c r="E28" s="20">
+        <v>2</v>
+      </c>
+      <c r="F28" s="21" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B28" s="49">
-        <v>2</v>
-      </c>
-      <c r="C28" s="56" t="s">
+    <row r="29" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B29" s="15">
+        <v>3</v>
+      </c>
+      <c r="C29" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="E28" s="28">
-        <v>2</v>
-      </c>
-      <c r="F28" s="29" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B29" s="18">
+      <c r="E29" s="20">
         <v>3</v>
       </c>
-      <c r="C29" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="E29" s="28">
-        <v>3</v>
-      </c>
-      <c r="F29" s="29" t="s">
-        <v>56</v>
+      <c r="F29" s="21" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B30" s="10"/>
       <c r="C30" s="9"/>
-      <c r="E30" s="28">
+      <c r="E30" s="20">
         <v>4</v>
       </c>
-      <c r="F30" s="29" t="s">
-        <v>57</v>
+      <c r="F30" s="21" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B31" s="10"/>
       <c r="C31" s="9"/>
-      <c r="E31" s="30">
+      <c r="E31" s="22">
         <v>5</v>
       </c>
-      <c r="F31" s="55" t="s">
-        <v>55</v>
+      <c r="F31" s="44" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B33" s="11" t="s">
+      <c r="B33" s="51" t="s">
         <v>20</v>
       </c>
-      <c r="C33" s="12"/>
-      <c r="D33" s="12"/>
-      <c r="E33" s="12"/>
-      <c r="F33" s="12"/>
-      <c r="G33" s="12"/>
-      <c r="H33" s="13"/>
+      <c r="C33" s="55"/>
+      <c r="D33" s="55"/>
+      <c r="E33" s="55"/>
+      <c r="F33" s="55"/>
+      <c r="G33" s="55"/>
+      <c r="H33" s="52"/>
     </row>
     <row r="34" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="14" t="s">
+      <c r="B34" s="11" t="s">
         <v>21</v>
       </c>
       <c r="C34" s="2" t="s">
@@ -1618,67 +1618,67 @@
       <c r="G34" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="H34" s="15" t="s">
+      <c r="H34" s="12" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="50">
-        <v>1</v>
-      </c>
-      <c r="C35" s="51">
-        <v>1</v>
-      </c>
-      <c r="D35" s="51">
-        <v>1</v>
-      </c>
-      <c r="E35" s="52">
+      <c r="B35" s="39">
+        <v>1</v>
+      </c>
+      <c r="C35" s="40">
+        <v>1</v>
+      </c>
+      <c r="D35" s="40">
+        <v>1</v>
+      </c>
+      <c r="E35" s="41">
         <v>43151</v>
       </c>
-      <c r="F35" s="53">
+      <c r="F35" s="42">
         <v>0.5</v>
       </c>
-      <c r="G35" s="51">
-        <v>1</v>
-      </c>
-      <c r="H35" s="54" t="s">
-        <v>52</v>
+      <c r="G35" s="40">
+        <v>1</v>
+      </c>
+      <c r="H35" s="43" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B36" s="16"/>
+      <c r="B36" s="13"/>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
       <c r="G36" s="3"/>
-      <c r="H36" s="17"/>
+      <c r="H36" s="14"/>
     </row>
     <row r="37" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B37" s="18"/>
-      <c r="C37" s="19"/>
-      <c r="D37" s="19"/>
-      <c r="E37" s="19"/>
-      <c r="F37" s="19"/>
-      <c r="G37" s="19"/>
-      <c r="H37" s="20"/>
+      <c r="B37" s="15"/>
+      <c r="C37" s="16"/>
+      <c r="D37" s="16"/>
+      <c r="E37" s="16"/>
+      <c r="F37" s="16"/>
+      <c r="G37" s="16"/>
+      <c r="H37" s="17"/>
     </row>
     <row r="38" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A39" s="37" t="s">
+      <c r="A39" s="56" t="s">
         <v>28</v>
       </c>
-      <c r="B39" s="12"/>
-      <c r="C39" s="12"/>
-      <c r="D39" s="12"/>
-      <c r="E39" s="13"/>
+      <c r="B39" s="55"/>
+      <c r="C39" s="55"/>
+      <c r="D39" s="55"/>
+      <c r="E39" s="52"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A40" s="26" t="s">
+      <c r="A40" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="B40" s="36" t="s">
-        <v>58</v>
+      <c r="B40" s="28" t="s">
+        <v>68</v>
       </c>
       <c r="C40" s="4" t="s">
         <v>29</v>
@@ -1686,54 +1686,54 @@
       <c r="D40" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="E40" s="35" t="s">
+      <c r="E40" s="27" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A41" s="28">
-        <v>1</v>
-      </c>
-      <c r="B41" s="39">
+      <c r="A41" s="20">
+        <v>1</v>
+      </c>
+      <c r="B41" s="30">
         <v>1</v>
       </c>
       <c r="C41" s="3">
         <v>1.56</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="E41" s="17" t="s">
-        <v>60</v>
+        <v>57</v>
+      </c>
+      <c r="E41" s="14" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A42" s="28"/>
-      <c r="B42" s="39"/>
+      <c r="A42" s="20"/>
+      <c r="B42" s="30"/>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
-      <c r="E42" s="17"/>
+      <c r="E42" s="14"/>
     </row>
     <row r="43" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="30"/>
-      <c r="B43" s="57"/>
-      <c r="C43" s="19"/>
-      <c r="D43" s="19"/>
-      <c r="E43" s="20"/>
+      <c r="A43" s="22"/>
+      <c r="B43" s="46"/>
+      <c r="C43" s="16"/>
+      <c r="D43" s="16"/>
+      <c r="E43" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="H12:K12"/>
-    <mergeCell ref="A12:F12"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="E7:F7"/>
     <mergeCell ref="B1:H1"/>
     <mergeCell ref="B25:C25"/>
     <mergeCell ref="B33:H33"/>
     <mergeCell ref="A39:E39"/>
     <mergeCell ref="A18:J18"/>
     <mergeCell ref="E25:F25"/>
+    <mergeCell ref="H12:K12"/>
+    <mergeCell ref="A12:F12"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="E7:F7"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="I14" r:id="rId1"/>

</xml_diff>

<commit_message>
Finalizados scripts de insercao e selecao no Banco de Dados
</commit_message>
<xml_diff>
--- a/Banco de Dados/SPMedGroup_TabelasValidacao.xlsx
+++ b/Banco de Dados/SPMedGroup_TabelasValidacao.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="73">
   <si>
     <t>Nome</t>
   </si>
@@ -234,13 +234,22 @@
   </si>
   <si>
     <t>médico</t>
+  </si>
+  <si>
+    <t>Id_Prontuário</t>
+  </si>
+  <si>
+    <t>Id_Consulta</t>
+  </si>
+  <si>
+    <t>PRONTUARIOS_CONSULTAS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -252,6 +261,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -665,7 +680,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -761,65 +776,74 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1102,10 +1126,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K43"/>
+  <dimension ref="A1:K51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F19" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1124,15 +1148,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
-      <c r="H1" s="50"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="45"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B2" s="18" t="s">
@@ -1176,7 +1200,7 @@
       <c r="G3" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="H3" s="47" t="s">
+      <c r="H3" s="42" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1200,18 +1224,18 @@
     </row>
     <row r="6" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B7" s="53" t="s">
+      <c r="B7" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="54"/>
-      <c r="E7" s="51" t="s">
+      <c r="C7" s="47"/>
+      <c r="E7" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="52"/>
-      <c r="H7" s="51" t="s">
+      <c r="F7" s="50"/>
+      <c r="H7" s="48" t="s">
         <v>67</v>
       </c>
-      <c r="I7" s="52"/>
+      <c r="I7" s="50"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B8" s="11" t="s">
@@ -1269,20 +1293,20 @@
     </row>
     <row r="11" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="48" t="s">
+      <c r="A12" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="49"/>
-      <c r="C12" s="49"/>
-      <c r="D12" s="49"/>
-      <c r="E12" s="49"/>
-      <c r="F12" s="50"/>
-      <c r="H12" s="48" t="s">
+      <c r="B12" s="44"/>
+      <c r="C12" s="44"/>
+      <c r="D12" s="44"/>
+      <c r="E12" s="44"/>
+      <c r="F12" s="45"/>
+      <c r="H12" s="43" t="s">
         <v>31</v>
       </c>
-      <c r="I12" s="49"/>
-      <c r="J12" s="49"/>
-      <c r="K12" s="50"/>
+      <c r="I12" s="44"/>
+      <c r="J12" s="44"/>
+      <c r="K12" s="45"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="18" t="s">
@@ -1386,18 +1410,18 @@
       <c r="D17" s="9"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A18" s="56" t="s">
+      <c r="A18" s="51" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="57"/>
-      <c r="C18" s="57"/>
-      <c r="D18" s="57"/>
-      <c r="E18" s="57"/>
-      <c r="F18" s="57"/>
-      <c r="G18" s="57"/>
-      <c r="H18" s="57"/>
-      <c r="I18" s="57"/>
-      <c r="J18" s="58"/>
+      <c r="B18" s="52"/>
+      <c r="C18" s="52"/>
+      <c r="D18" s="52"/>
+      <c r="E18" s="52"/>
+      <c r="F18" s="52"/>
+      <c r="G18" s="52"/>
+      <c r="H18" s="52"/>
+      <c r="I18" s="52"/>
+      <c r="J18" s="53"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="18" t="s">
@@ -1490,7 +1514,7 @@
     </row>
     <row r="23" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="34"/>
-      <c r="B23" s="46"/>
+      <c r="B23" s="41"/>
       <c r="C23" s="35"/>
       <c r="D23" s="35"/>
       <c r="E23" s="35"/>
@@ -1502,14 +1526,14 @@
     </row>
     <row r="24" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B25" s="53" t="s">
+      <c r="B25" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="C25" s="54"/>
-      <c r="E25" s="48" t="s">
+      <c r="C25" s="47"/>
+      <c r="E25" s="43" t="s">
         <v>66</v>
       </c>
-      <c r="F25" s="50"/>
+      <c r="F25" s="45"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B26" s="11" t="s">
@@ -1543,7 +1567,7 @@
       <c r="B28" s="38">
         <v>2</v>
       </c>
-      <c r="C28" s="45" t="s">
+      <c r="C28" s="40" t="s">
         <v>49</v>
       </c>
       <c r="E28" s="20">
@@ -1583,95 +1607,103 @@
       <c r="E31" s="22">
         <v>5</v>
       </c>
-      <c r="F31" s="44" t="s">
+      <c r="F31" s="39" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B33" s="51" t="s">
+      <c r="A33" s="54" t="s">
         <v>20</v>
       </c>
-      <c r="C33" s="55"/>
-      <c r="D33" s="55"/>
-      <c r="E33" s="55"/>
-      <c r="F33" s="55"/>
-      <c r="G33" s="55"/>
-      <c r="H33" s="52"/>
+      <c r="B33" s="54"/>
+      <c r="C33" s="54"/>
+      <c r="D33" s="54"/>
+      <c r="E33" s="54"/>
+      <c r="F33" s="54"/>
+      <c r="G33" s="54"/>
+      <c r="H33" s="54"/>
     </row>
     <row r="34" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="11" t="s">
+      <c r="A34" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="B34" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="C34" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="D34" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E34" s="2" t="s">
+      <c r="E34" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F34" s="2" t="s">
+      <c r="F34" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G34" s="2" t="s">
+      <c r="G34" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="H34" s="12" t="s">
+      <c r="H34" s="5" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="39">
-        <v>1</v>
-      </c>
-      <c r="C35" s="40">
-        <v>1</v>
-      </c>
-      <c r="D35" s="40">
-        <v>1</v>
-      </c>
-      <c r="E35" s="41">
+      <c r="A35" s="55">
+        <v>1</v>
+      </c>
+      <c r="B35" s="55">
+        <v>1</v>
+      </c>
+      <c r="C35" s="55">
+        <v>1</v>
+      </c>
+      <c r="D35" s="55">
+        <v>1</v>
+      </c>
+      <c r="E35" s="56">
         <v>43151</v>
       </c>
-      <c r="F35" s="42">
+      <c r="F35" s="57">
         <v>0.5</v>
       </c>
-      <c r="G35" s="40">
-        <v>1</v>
-      </c>
-      <c r="H35" s="43" t="s">
+      <c r="G35" s="55">
+        <v>1</v>
+      </c>
+      <c r="H35" s="58" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B36" s="13"/>
-      <c r="C36" s="3"/>
-      <c r="D36" s="3"/>
-      <c r="E36" s="3"/>
-      <c r="F36" s="3"/>
-      <c r="G36" s="3"/>
-      <c r="H36" s="14"/>
-    </row>
-    <row r="37" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B37" s="15"/>
-      <c r="C37" s="16"/>
-      <c r="D37" s="16"/>
-      <c r="E37" s="16"/>
-      <c r="F37" s="16"/>
-      <c r="G37" s="16"/>
-      <c r="H37" s="17"/>
+      <c r="A36" s="6"/>
+      <c r="B36" s="8"/>
+      <c r="C36" s="8"/>
+      <c r="D36" s="8"/>
+      <c r="E36" s="8"/>
+      <c r="F36" s="8"/>
+      <c r="G36" s="8"/>
+      <c r="H36" s="8"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A37" s="6"/>
+      <c r="B37" s="8"/>
+      <c r="C37" s="8"/>
+      <c r="D37" s="8"/>
+      <c r="E37" s="8"/>
+      <c r="F37" s="8"/>
+      <c r="G37" s="8"/>
+      <c r="H37" s="8"/>
     </row>
     <row r="38" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A39" s="56" t="s">
+      <c r="A39" s="51" t="s">
         <v>28</v>
       </c>
-      <c r="B39" s="55"/>
-      <c r="C39" s="55"/>
-      <c r="D39" s="55"/>
-      <c r="E39" s="52"/>
+      <c r="B39" s="49"/>
+      <c r="C39" s="49"/>
+      <c r="D39" s="49"/>
+      <c r="E39" s="50"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" s="18" t="s">
@@ -1689,6 +1721,7 @@
       <c r="E40" s="27" t="s">
         <v>27</v>
       </c>
+      <c r="F40" s="61"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" s="20">
@@ -1706,6 +1739,7 @@
       <c r="E41" s="14" t="s">
         <v>58</v>
       </c>
+      <c r="F41" s="60"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" s="20"/>
@@ -1716,16 +1750,55 @@
     </row>
     <row r="43" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="22"/>
-      <c r="B43" s="46"/>
+      <c r="B43" s="41"/>
       <c r="C43" s="16"/>
       <c r="D43" s="16"/>
       <c r="E43" s="17"/>
     </row>
+    <row r="46" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A47" s="51" t="s">
+        <v>72</v>
+      </c>
+      <c r="B47" s="53"/>
+    </row>
+    <row r="48" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49" s="55">
+        <v>1</v>
+      </c>
+      <c r="B49" s="55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50" s="55">
+        <v>1</v>
+      </c>
+      <c r="B50" s="55">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51" s="55">
+        <v>1</v>
+      </c>
+      <c r="B51" s="55">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="12">
+    <mergeCell ref="A47:B47"/>
     <mergeCell ref="B1:H1"/>
     <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B33:H33"/>
     <mergeCell ref="A39:E39"/>
     <mergeCell ref="A18:J18"/>
     <mergeCell ref="E25:F25"/>
@@ -1734,11 +1807,13 @@
     <mergeCell ref="H7:I7"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="E7:F7"/>
+    <mergeCell ref="A33:H33"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="I14" r:id="rId1"/>
     <hyperlink ref="I15" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>